<commit_message>
adjusted spending for inflation, added correlation tables, and added a page for findings
</commit_message>
<xml_diff>
--- a/drug_war/drug_control_spending_1995_2018_copy.xlsx
+++ b/drug_war/drug_control_spending_1995_2018_copy.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliasabunuwara/Desktop/Courses/Spring_2020/GOV_1005/final_project/raw_data/usa/charts/budget_reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliasabunuwara/Desktop/Courses/Spring_2020/GOV_1005/drug_war_final_project/drug_war/drug_war/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7353555C-92C0-554C-9EA4-D2FC84660529}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81405011-3A2D-5844-AE65-CDCDBBDE7CEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="21000" xr2:uid="{B900A2C6-163F-F84F-94AA-28511E8F4B73}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22980" windowHeight="19440" xr2:uid="{B900A2C6-163F-F84F-94AA-28511E8F4B73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>year</t>
   </si>
@@ -46,15 +46,25 @@
   <si>
     <t>total</t>
   </si>
+  <si>
+    <t>adjusted_2020</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF330000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,19 +407,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EC851A-EF9D-2446-9EE1-415D0813EDD8}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,8 +433,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1995</v>
       </c>
@@ -435,8 +450,11 @@
       <c r="D2">
         <v>7045.6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="1">
+        <v>12092.88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1996</v>
       </c>
@@ -450,8 +468,11 @@
       <c r="D3">
         <v>6808.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="1">
+        <v>11375.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1997</v>
       </c>
@@ -465,8 +486,11 @@
       <c r="D4">
         <v>8090.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="1">
+        <v>13118.42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1998</v>
       </c>
@@ -480,8 +504,11 @@
       <c r="D5">
         <v>8179</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="1">
+        <v>13056.59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1999</v>
       </c>
@@ -495,8 +522,11 @@
       <c r="D6">
         <v>9760.1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="1">
+        <v>15324.55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2000</v>
       </c>
@@ -510,8 +540,11 @@
       <c r="D7">
         <v>10703</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="1">
+        <v>16357.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2001</v>
       </c>
@@ -525,8 +558,11 @@
       <c r="D8">
         <v>10401.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="1">
+        <v>15324.16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2002</v>
       </c>
@@ -540,8 +576,11 @@
       <c r="D9">
         <v>10781.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="1">
+        <v>15704.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2003</v>
       </c>
@@ -555,8 +594,11 @@
         <f>SUM(B10:C10)</f>
         <v>17053.400000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="1">
+        <v>24211.79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2004</v>
       </c>
@@ -570,8 +612,11 @@
         <f t="shared" ref="D11:D26" si="1">SUM(B11:C11)</f>
         <v>18556</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="1">
+        <v>25847.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2005</v>
       </c>
@@ -585,8 +630,11 @@
         <f t="shared" si="1"/>
         <v>19881.7</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="1">
+        <v>26895.13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2006</v>
       </c>
@@ -600,8 +648,11 @@
         <f t="shared" si="1"/>
         <v>20613.900000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="1">
+        <v>26816.89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2007</v>
       </c>
@@ -615,8 +666,11 @@
         <f>SUM(B14:C14)</f>
         <v>21683.599999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="1">
+        <v>27634.87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2008</v>
       </c>
@@ -630,8 +684,11 @@
         <f t="shared" si="1"/>
         <v>21834.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="1">
+        <v>26684.62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2009</v>
       </c>
@@ -642,11 +699,14 @@
         <v>15701.9</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f>SUM(B16:C16)</f>
         <v>24864.6</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="1">
+        <v>30379.15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2010</v>
       </c>
@@ -657,11 +717,14 @@
         <v>15509.9</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f>SUM(B17:C17)</f>
         <v>24620.799999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="1">
+        <v>29311.64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2011</v>
       </c>
@@ -675,8 +738,11 @@
         <f t="shared" si="1"/>
         <v>24365.4</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="1">
+        <v>28541.83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2012</v>
       </c>
@@ -690,8 +756,11 @@
         <f t="shared" si="1"/>
         <v>24504.1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="1">
+        <v>27888.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2013</v>
       </c>
@@ -705,8 +774,11 @@
         <f t="shared" si="1"/>
         <v>23809.599999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="1">
+        <v>26672.69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2014</v>
       </c>
@@ -720,8 +792,11 @@
         <f t="shared" si="1"/>
         <v>25733.1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="1">
+        <v>28379.39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2015</v>
       </c>
@@ -735,8 +810,11 @@
         <f t="shared" si="1"/>
         <v>25892.9</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="1">
+        <v>28581.16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2016</v>
       </c>
@@ -750,8 +828,11 @@
         <f t="shared" si="1"/>
         <v>26874</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="1">
+        <v>29262.32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2017</v>
       </c>
@@ -765,8 +846,11 @@
         <f t="shared" si="1"/>
         <v>28813.3</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="1">
+        <v>30608.74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2018</v>
       </c>
@@ -780,8 +864,11 @@
         <f t="shared" si="1"/>
         <v>33286.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="1">
+        <v>34643.379999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -794,6 +881,9 @@
       <c r="D26">
         <f t="shared" si="1"/>
         <v>36808.300000000003</v>
+      </c>
+      <c r="E26" s="1">
+        <v>37723.56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>